<commit_message>
added some fish data from dave and made some example GLM code
</commit_message>
<xml_diff>
--- a/blitz2/zoocodes.xlsx
+++ b/blitz2/zoocodes.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rkhartman\Documents\Documents\phaseIV\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rkhartman\Documents\Documents\FRPreport2018\blitz2\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -4603,17 +4603,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N530"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C521" sqref="C521"/>
+    <sheetView tabSelected="1" topLeftCell="A249" workbookViewId="0">
+      <selection activeCell="O257" sqref="O257"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="20.140625" customWidth="1"/>
+    <col min="3" max="3" width="20.109375" customWidth="1"/>
     <col min="13" max="13" width="12" customWidth="1"/>
+    <col min="14" max="14" width="29.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1354</v>
       </c>
@@ -4657,7 +4658,7 @@
         <v>1358</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>78</v>
       </c>
@@ -4701,7 +4702,7 @@
         <v>1362</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>112</v>
       </c>
@@ -4745,7 +4746,7 @@
         <v>1363</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>150</v>
       </c>
@@ -4789,7 +4790,7 @@
         <v>1363</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>267</v>
       </c>
@@ -4833,7 +4834,7 @@
         <v>1362</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>300</v>
       </c>
@@ -4878,7 +4879,7 @@
         <v>Americorophium spinicorne</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>301</v>
       </c>
@@ -4923,7 +4924,7 @@
         <v>Americorophium stimpsoni</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>302</v>
       </c>
@@ -4967,7 +4968,7 @@
         <v>1362</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>1</v>
       </c>
@@ -5011,7 +5012,7 @@
         <v>1359</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>101</v>
       </c>
@@ -5055,7 +5056,7 @@
         <v>1364</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>102</v>
       </c>
@@ -5100,7 +5101,7 @@
         <v>Oligocheate</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>180</v>
       </c>
@@ -5144,7 +5145,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>217</v>
       </c>
@@ -5188,7 +5189,7 @@
         <v>1365</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>220</v>
       </c>
@@ -5232,7 +5233,7 @@
         <v>1365</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>227</v>
       </c>
@@ -5276,7 +5277,7 @@
         <v>1366</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>105</v>
       </c>
@@ -5320,7 +5321,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>106</v>
       </c>
@@ -5364,7 +5365,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>204</v>
       </c>
@@ -5408,7 +5409,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>8</v>
       </c>
@@ -5452,7 +5453,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="20" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>139</v>
       </c>
@@ -5496,7 +5497,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <v>141</v>
       </c>
@@ -5540,7 +5541,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <v>245</v>
       </c>
@@ -5584,7 +5585,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="23" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <v>10003</v>
       </c>
@@ -5628,7 +5629,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="24" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <v>10012</v>
       </c>
@@ -5672,7 +5673,7 @@
         <v>1353</v>
       </c>
     </row>
-    <row r="25" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <v>31</v>
       </c>
@@ -5717,7 +5718,7 @@
         <v>Acartia spp.</v>
       </c>
     </row>
-    <row r="26" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <v>32</v>
       </c>
@@ -5762,7 +5763,7 @@
         <v>Diaptomidae spp.</v>
       </c>
     </row>
-    <row r="27" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
         <v>33</v>
       </c>
@@ -5807,7 +5808,7 @@
         <v>Pseudodiaptomus spp.</v>
       </c>
     </row>
-    <row r="28" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
         <v>34</v>
       </c>
@@ -5852,7 +5853,7 @@
         <v>Eurytemora affinis</v>
       </c>
     </row>
-    <row r="29" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
         <v>35</v>
       </c>
@@ -5897,7 +5898,7 @@
         <v>Sinocalanus</v>
       </c>
     </row>
-    <row r="30" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
         <v>36</v>
       </c>
@@ -5942,7 +5943,7 @@
         <v>Osphranticum</v>
       </c>
     </row>
-    <row r="31" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
         <v>37</v>
       </c>
@@ -5987,7 +5988,7 @@
         <v>Acartiella</v>
       </c>
     </row>
-    <row r="32" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
         <v>38</v>
       </c>
@@ -6032,7 +6033,7 @@
         <v>Tortanus</v>
       </c>
     </row>
-    <row r="33" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A33" s="2">
         <v>39</v>
       </c>
@@ -6077,7 +6078,7 @@
         <v>Acartia copepodid</v>
       </c>
     </row>
-    <row r="34" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A34" s="2">
         <v>40</v>
       </c>
@@ -6122,7 +6123,7 @@
         <v>calanoid copepodid</v>
       </c>
     </row>
-    <row r="35" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A35" s="2">
         <v>41</v>
       </c>
@@ -6167,7 +6168,7 @@
         <v>Eurytemora copepodid</v>
       </c>
     </row>
-    <row r="36" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A36" s="2">
         <v>42</v>
       </c>
@@ -6212,7 +6213,7 @@
         <v>Pseudodiaptomus copepodid</v>
       </c>
     </row>
-    <row r="37" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A37" s="2">
         <v>43</v>
       </c>
@@ -6257,7 +6258,7 @@
         <v>Pseudodiaptomus euryhalinus</v>
       </c>
     </row>
-    <row r="38" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A38" s="2">
         <v>44</v>
       </c>
@@ -6302,7 +6303,7 @@
         <v>Diaptomidae copepodid</v>
       </c>
     </row>
-    <row r="39" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A39" s="2">
         <v>45</v>
       </c>
@@ -6347,7 +6348,7 @@
         <v>Acartiella copepodid</v>
       </c>
     </row>
-    <row r="40" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A40" s="2">
         <v>46</v>
       </c>
@@ -6392,7 +6393,7 @@
         <v>Tortanus copepodid</v>
       </c>
     </row>
-    <row r="41" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A41" s="2">
         <v>47</v>
       </c>
@@ -6437,7 +6438,7 @@
         <v>Tortanus dextrilobatus</v>
       </c>
     </row>
-    <row r="42" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A42" s="2">
         <v>48</v>
       </c>
@@ -6482,7 +6483,7 @@
         <v>Calanoid UNID/other</v>
       </c>
     </row>
-    <row r="43" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A43" s="2">
         <v>49</v>
       </c>
@@ -6527,7 +6528,7 @@
         <v>Calanoid Other</v>
       </c>
     </row>
-    <row r="44" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A44" s="2">
         <v>50</v>
       </c>
@@ -6572,7 +6573,7 @@
         <v>Tortanus discaudatus</v>
       </c>
     </row>
-    <row r="45" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A45" s="2">
         <v>80</v>
       </c>
@@ -6617,7 +6618,7 @@
         <v>Eurytemora nauplii</v>
       </c>
     </row>
-    <row r="46" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A46" s="2">
         <v>81</v>
       </c>
@@ -6662,7 +6663,7 @@
         <v>Sinocalanus nauplii</v>
       </c>
     </row>
-    <row r="47" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A47" s="2">
         <v>82</v>
       </c>
@@ -6707,7 +6708,7 @@
         <v>Pseudodiaptomus nauplii</v>
       </c>
     </row>
-    <row r="48" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A48" s="2">
         <v>83</v>
       </c>
@@ -6752,7 +6753,7 @@
         <v>Sinocalanus copepodid</v>
       </c>
     </row>
-    <row r="49" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A49" s="2">
         <v>86</v>
       </c>
@@ -6797,7 +6798,7 @@
         <v>Pseudodiaptomus forbesii</v>
       </c>
     </row>
-    <row r="50" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A50" s="2">
         <v>87</v>
       </c>
@@ -6842,7 +6843,7 @@
         <v>Pseudodiaptomus marinus</v>
       </c>
     </row>
-    <row r="51" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A51" s="2">
         <v>108</v>
       </c>
@@ -6887,7 +6888,7 @@
         <v>Calanoid</v>
       </c>
     </row>
-    <row r="52" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A52" s="2">
         <v>304</v>
       </c>
@@ -6932,7 +6933,7 @@
         <v>Eurytemora (gravid)</v>
       </c>
     </row>
-    <row r="53" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A53" s="2">
         <v>305</v>
       </c>
@@ -6977,7 +6978,7 @@
         <v>P. forbesi (gravid)</v>
       </c>
     </row>
-    <row r="54" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A54" s="2">
         <v>306</v>
       </c>
@@ -7022,7 +7023,7 @@
         <v>Sinocalanus (gravid)</v>
       </c>
     </row>
-    <row r="55" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A55" s="2">
         <v>307</v>
       </c>
@@ -7067,7 +7068,7 @@
         <v>Osphranticum (gravid)</v>
       </c>
     </row>
-    <row r="56" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A56" s="2">
         <v>308</v>
       </c>
@@ -7112,7 +7113,7 @@
         <v>Diaptomidae (gravid)</v>
       </c>
     </row>
-    <row r="57" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A57" s="2">
         <v>309</v>
       </c>
@@ -7157,7 +7158,7 @@
         <v>P. marinus (gravid)</v>
       </c>
     </row>
-    <row r="58" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A58" s="2">
         <v>310</v>
       </c>
@@ -7202,7 +7203,7 @@
         <v>Calanoid copepod (gravid)</v>
       </c>
     </row>
-    <row r="59" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A59" s="2">
         <v>61</v>
       </c>
@@ -7247,7 +7248,7 @@
         <v>Bosmina</v>
       </c>
     </row>
-    <row r="60" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A60" s="2">
         <v>62</v>
       </c>
@@ -7292,7 +7293,7 @@
         <v>Daphnia</v>
       </c>
     </row>
-    <row r="61" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A61" s="2">
         <v>63</v>
       </c>
@@ -7337,7 +7338,7 @@
         <v>Diaphanosoma</v>
       </c>
     </row>
-    <row r="62" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A62" s="2">
         <v>64</v>
       </c>
@@ -7382,7 +7383,7 @@
         <v>Ceriodaphnia</v>
       </c>
     </row>
-    <row r="63" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A63" s="2">
         <v>69</v>
       </c>
@@ -7427,7 +7428,7 @@
         <v>cladocera other</v>
       </c>
     </row>
-    <row r="64" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A64" s="2">
         <v>107</v>
       </c>
@@ -7472,7 +7473,7 @@
         <v>Cladocera</v>
       </c>
     </row>
-    <row r="65" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A65" s="2">
         <v>250</v>
       </c>
@@ -7517,7 +7518,7 @@
         <v>Chydorus</v>
       </c>
     </row>
-    <row r="66" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A66" s="2">
         <v>251</v>
       </c>
@@ -7562,7 +7563,7 @@
         <v>Moina</v>
       </c>
     </row>
-    <row r="67" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A67" s="2">
         <v>252</v>
       </c>
@@ -7607,7 +7608,7 @@
         <v>Sida</v>
       </c>
     </row>
-    <row r="68" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A68" s="2">
         <v>255</v>
       </c>
@@ -7652,7 +7653,7 @@
         <v>Simocephalus</v>
       </c>
     </row>
-    <row r="69" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A69" s="2">
         <v>257</v>
       </c>
@@ -7697,7 +7698,7 @@
         <v>Ilyocryptus</v>
       </c>
     </row>
-    <row r="70" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A70" s="2">
         <v>258</v>
       </c>
@@ -7742,7 +7743,7 @@
         <v>Scapholeberis</v>
       </c>
     </row>
-    <row r="71" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A71" s="2">
         <v>265</v>
       </c>
@@ -7787,7 +7788,7 @@
         <v>Holopedium</v>
       </c>
     </row>
-    <row r="72" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A72" s="2">
         <v>266</v>
       </c>
@@ -7832,7 +7833,7 @@
         <v>Macrothricidae</v>
       </c>
     </row>
-    <row r="73" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A73" s="2">
         <v>268</v>
       </c>
@@ -7877,7 +7878,7 @@
         <v>Leptodora</v>
       </c>
     </row>
-    <row r="74" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A74" s="2">
         <v>269</v>
       </c>
@@ -7922,7 +7923,7 @@
         <v>Latona</v>
       </c>
     </row>
-    <row r="75" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A75" s="2">
         <v>137</v>
       </c>
@@ -7967,7 +7968,7 @@
         <v>Hydra</v>
       </c>
     </row>
-    <row r="76" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A76" s="2">
         <v>138</v>
       </c>
@@ -8011,7 +8012,7 @@
         <v>1353</v>
       </c>
     </row>
-    <row r="77" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A77" s="2">
         <v>113</v>
       </c>
@@ -8055,7 +8056,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="78" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A78" s="2">
         <v>157</v>
       </c>
@@ -8099,7 +8100,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="79" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A79" s="2">
         <v>160</v>
       </c>
@@ -8143,7 +8144,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="80" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A80" s="2">
         <v>167</v>
       </c>
@@ -8187,7 +8188,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="81" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A81" s="2">
         <v>174</v>
       </c>
@@ -8231,7 +8232,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="82" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A82" s="2">
         <v>183</v>
       </c>
@@ -8275,7 +8276,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="83" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A83" s="2">
         <v>188</v>
       </c>
@@ -8319,7 +8320,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="84" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A84" s="2">
         <v>201</v>
       </c>
@@ -8363,7 +8364,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="85" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A85" s="2">
         <v>202</v>
       </c>
@@ -8407,7 +8408,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="86" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A86" s="2">
         <v>203</v>
       </c>
@@ -8451,7 +8452,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="87" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A87" s="2">
         <v>213</v>
       </c>
@@ -8495,7 +8496,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="88" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A88" s="2">
         <v>215</v>
       </c>
@@ -8539,7 +8540,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="89" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A89" s="2">
         <v>230</v>
       </c>
@@ -8583,7 +8584,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="90" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A90" s="2">
         <v>233</v>
       </c>
@@ -8627,7 +8628,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="91" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A91" s="2">
         <v>234</v>
       </c>
@@ -8671,7 +8672,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="92" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A92" s="2">
         <v>235</v>
       </c>
@@ -8715,7 +8716,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="93" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A93" s="2">
         <v>239</v>
       </c>
@@ -8759,7 +8760,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="94" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A94" s="2">
         <v>10002</v>
       </c>
@@ -8803,7 +8804,7 @@
         <v>1367</v>
       </c>
     </row>
-    <row r="95" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A95" s="2">
         <v>10006</v>
       </c>
@@ -8847,7 +8848,7 @@
         <v>1310</v>
       </c>
     </row>
-    <row r="96" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A96" s="2">
         <v>10007</v>
       </c>
@@ -8891,7 +8892,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="97" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A97" s="2">
         <v>104</v>
       </c>
@@ -8935,7 +8936,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="98" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A98" s="2">
         <v>72</v>
       </c>
@@ -8979,7 +8980,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="99" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A99" s="2">
         <v>20</v>
       </c>
@@ -9024,7 +9025,7 @@
         <v>Cyclopoid copepodid</v>
       </c>
     </row>
-    <row r="100" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A100" s="2">
         <v>21</v>
       </c>
@@ -9069,7 +9070,7 @@
         <v>Acanthocyclops</v>
       </c>
     </row>
-    <row r="101" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A101" s="2">
         <v>22</v>
       </c>
@@ -9114,7 +9115,7 @@
         <v>Oithona similis</v>
       </c>
     </row>
-    <row r="102" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A102" s="2">
         <v>23</v>
       </c>
@@ -9159,7 +9160,7 @@
         <v>Oithona davisae</v>
       </c>
     </row>
-    <row r="103" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A103" s="2">
         <v>24</v>
       </c>
@@ -9204,7 +9205,7 @@
         <v>Limnoithona spp.</v>
       </c>
     </row>
-    <row r="104" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A104" s="2">
         <v>25</v>
       </c>
@@ -9249,7 +9250,7 @@
         <v>Limnoithona sinensis</v>
       </c>
     </row>
-    <row r="105" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A105" s="2">
         <v>26</v>
       </c>
@@ -9294,7 +9295,7 @@
         <v>Limnoithona tetraspina</v>
       </c>
     </row>
-    <row r="106" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A106" s="2">
         <v>27</v>
       </c>
@@ -9339,7 +9340,7 @@
         <v>Oithona spp.</v>
       </c>
     </row>
-    <row r="107" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A107" s="2">
         <v>28</v>
       </c>
@@ -9384,7 +9385,7 @@
         <v>Cyclopoid UNID</v>
       </c>
     </row>
-    <row r="108" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A108" s="2">
         <v>29</v>
       </c>
@@ -9429,7 +9430,7 @@
         <v>Cyclopoid Other</v>
       </c>
     </row>
-    <row r="109" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A109" s="2">
         <v>84</v>
       </c>
@@ -9474,7 +9475,7 @@
         <v>Limnoithona juvenile</v>
       </c>
     </row>
-    <row r="110" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A110" s="2">
         <v>85</v>
       </c>
@@ -9519,7 +9520,7 @@
         <v>Oithona juvenile</v>
       </c>
     </row>
-    <row r="111" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A111" s="2">
         <v>109</v>
       </c>
@@ -9564,7 +9565,7 @@
         <v>Cyclopoid</v>
       </c>
     </row>
-    <row r="112" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A112" s="2">
         <v>247</v>
       </c>
@@ -9609,7 +9610,7 @@
         <v>Halicyclops</v>
       </c>
     </row>
-    <row r="113" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A113" s="2">
         <v>248</v>
       </c>
@@ -9654,7 +9655,7 @@
         <v>Diacyclops</v>
       </c>
     </row>
-    <row r="114" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A114" s="2">
         <v>259</v>
       </c>
@@ -9699,7 +9700,7 @@
         <v>Eucyclops</v>
       </c>
     </row>
-    <row r="115" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A115" s="2">
         <v>261</v>
       </c>
@@ -9744,7 +9745,7 @@
         <v>Macrocyclops</v>
       </c>
     </row>
-    <row r="116" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A116" s="2">
         <v>262</v>
       </c>
@@ -9789,7 +9790,7 @@
         <v>Homocyclops</v>
       </c>
     </row>
-    <row r="117" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A117" s="2">
         <v>263</v>
       </c>
@@ -9834,7 +9835,7 @@
         <v>Mesocyclops</v>
       </c>
     </row>
-    <row r="118" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A118" s="2">
         <v>311</v>
       </c>
@@ -9879,7 +9880,7 @@
         <v>Paracyclops</v>
       </c>
     </row>
-    <row r="119" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A119" s="2">
         <v>316</v>
       </c>
@@ -9924,7 +9925,7 @@
         <v>Microcyclops</v>
       </c>
     </row>
-    <row r="120" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A120" s="2">
         <v>74</v>
       </c>
@@ -9969,7 +9970,7 @@
         <v>crab zoea</v>
       </c>
     </row>
-    <row r="121" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A121" s="2">
         <v>75</v>
       </c>
@@ -10014,7 +10015,7 @@
         <v>Palaemon</v>
       </c>
     </row>
-    <row r="122" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A122" s="2">
         <v>76</v>
       </c>
@@ -10059,7 +10060,7 @@
         <v>Crangon</v>
       </c>
     </row>
-    <row r="123" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A123" s="2">
         <v>94</v>
       </c>
@@ -10104,7 +10105,7 @@
         <v>Crab megalope</v>
       </c>
     </row>
-    <row r="124" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A124" s="2">
         <v>136</v>
       </c>
@@ -10149,7 +10150,7 @@
         <v>Exopalaemon</v>
       </c>
     </row>
-    <row r="125" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A125" s="2">
         <v>156</v>
       </c>
@@ -10194,7 +10195,7 @@
         <v>Shrimp Other</v>
       </c>
     </row>
-    <row r="126" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A126" s="2">
         <v>171</v>
       </c>
@@ -10239,7 +10240,7 @@
         <v>Crayfish</v>
       </c>
     </row>
-    <row r="127" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A127" s="2">
         <v>216</v>
       </c>
@@ -10284,7 +10285,7 @@
         <v>Palaemonetes</v>
       </c>
     </row>
-    <row r="128" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A128" s="2">
         <v>224</v>
       </c>
@@ -10329,7 +10330,7 @@
         <v>Shrimp juvenile</v>
       </c>
     </row>
-    <row r="129" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A129" s="2">
         <v>193</v>
       </c>
@@ -10373,7 +10374,7 @@
         <v>1353</v>
       </c>
     </row>
-    <row r="130" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A130" s="2">
         <v>3</v>
       </c>
@@ -10417,7 +10418,7 @@
         <v>1361</v>
       </c>
     </row>
-    <row r="131" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A131" s="2">
         <v>115</v>
       </c>
@@ -10461,7 +10462,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="132" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A132" s="2">
         <v>116</v>
       </c>
@@ -10505,7 +10506,7 @@
         <v>1368</v>
       </c>
     </row>
-    <row r="133" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A133" s="2">
         <v>155</v>
       </c>
@@ -10549,7 +10550,7 @@
         <v>1373</v>
       </c>
     </row>
-    <row r="134" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A134" s="2">
         <v>158</v>
       </c>
@@ -10593,7 +10594,7 @@
         <v>1373</v>
       </c>
     </row>
-    <row r="135" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A135" s="2">
         <v>165</v>
       </c>
@@ -10637,7 +10638,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="136" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A136" s="2">
         <v>173</v>
       </c>
@@ -10681,7 +10682,7 @@
         <v>1373</v>
       </c>
     </row>
-    <row r="137" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A137" s="2">
         <v>179</v>
       </c>
@@ -10725,7 +10726,7 @@
         <v>1373</v>
       </c>
     </row>
-    <row r="138" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A138" s="2">
         <v>187</v>
       </c>
@@ -10769,7 +10770,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="139" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A139" s="2">
         <v>192</v>
       </c>
@@ -10814,7 +10815,7 @@
         <v>Tabanidae</v>
       </c>
     </row>
-    <row r="140" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A140" s="2">
         <v>194</v>
       </c>
@@ -10858,7 +10859,7 @@
         <v>1373</v>
       </c>
     </row>
-    <row r="141" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A141" s="2">
         <v>208</v>
       </c>
@@ -10903,7 +10904,7 @@
         <v>Dolichopodidae</v>
       </c>
     </row>
-    <row r="142" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A142" s="2">
         <v>210</v>
       </c>
@@ -10947,7 +10948,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="143" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A143" s="2">
         <v>211</v>
       </c>
@@ -10991,7 +10992,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="144" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A144" s="2">
         <v>229</v>
       </c>
@@ -11035,7 +11036,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="145" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A145" s="2">
         <v>232</v>
       </c>
@@ -11079,7 +11080,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="146" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A146" s="2">
         <v>10010</v>
       </c>
@@ -11123,7 +11124,7 @@
         <v>1315</v>
       </c>
     </row>
-    <row r="147" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A147" s="2">
         <v>10011</v>
       </c>
@@ -11167,7 +11168,7 @@
         <v>1315</v>
       </c>
     </row>
-    <row r="148" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A148" s="2">
         <v>10020</v>
       </c>
@@ -11212,7 +11213,7 @@
         <v>Hydroscaphidae</v>
       </c>
     </row>
-    <row r="149" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A149" s="2">
         <v>117</v>
       </c>
@@ -11257,7 +11258,7 @@
         <v>Baetidae</v>
       </c>
     </row>
-    <row r="150" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A150" s="2">
         <v>118</v>
       </c>
@@ -11302,7 +11303,7 @@
         <v>Caenidae</v>
       </c>
     </row>
-    <row r="151" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A151" s="2">
         <v>119</v>
       </c>
@@ -11346,7 +11347,7 @@
         <v>1374</v>
       </c>
     </row>
-    <row r="152" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A152" s="2">
         <v>168</v>
       </c>
@@ -11390,7 +11391,7 @@
         <v>1374</v>
       </c>
     </row>
-    <row r="153" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A153" s="2">
         <v>205</v>
       </c>
@@ -11434,7 +11435,7 @@
         <v>1374</v>
       </c>
     </row>
-    <row r="154" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A154" s="2">
         <v>206</v>
       </c>
@@ -11478,7 +11479,7 @@
         <v>1374</v>
       </c>
     </row>
-    <row r="155" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A155" s="2">
         <v>242</v>
       </c>
@@ -11522,7 +11523,7 @@
         <v>1374</v>
       </c>
     </row>
-    <row r="156" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A156" s="2">
         <v>5</v>
       </c>
@@ -11566,7 +11567,7 @@
         <v>1348</v>
       </c>
     </row>
-    <row r="157" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A157" s="2">
         <v>6</v>
       </c>
@@ -11610,7 +11611,7 @@
         <v>1348</v>
       </c>
     </row>
-    <row r="158" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A158" s="2">
         <v>153</v>
       </c>
@@ -11654,7 +11655,7 @@
         <v>1369</v>
       </c>
     </row>
-    <row r="159" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A159" s="2">
         <v>164</v>
       </c>
@@ -11699,7 +11700,7 @@
         <v>Mosquitofish</v>
       </c>
     </row>
-    <row r="160" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A160" s="2">
         <v>175</v>
       </c>
@@ -11744,7 +11745,7 @@
         <v>Sacramento Sucker</v>
       </c>
     </row>
-    <row r="161" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A161" s="2">
         <v>177</v>
       </c>
@@ -11789,7 +11790,7 @@
         <v>Prickly Sculpin</v>
       </c>
     </row>
-    <row r="162" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A162" s="2">
         <v>186</v>
       </c>
@@ -11834,7 +11835,7 @@
         <v>Rainwater Killifish</v>
       </c>
     </row>
-    <row r="163" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A163" s="2">
         <v>195</v>
       </c>
@@ -11879,7 +11880,7 @@
         <v>Fish larvae</v>
       </c>
     </row>
-    <row r="164" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A164" s="2">
         <v>197</v>
       </c>
@@ -11924,7 +11925,7 @@
         <v>Mississippi Silverside</v>
       </c>
     </row>
-    <row r="165" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A165" s="2">
         <v>238</v>
       </c>
@@ -11969,7 +11970,7 @@
         <v>Striped Bass</v>
       </c>
     </row>
-    <row r="166" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A166" s="2">
         <v>902</v>
       </c>
@@ -12012,7 +12013,7 @@
         <v>American Shad</v>
       </c>
     </row>
-    <row r="167" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A167" s="2">
         <v>903</v>
       </c>
@@ -12055,7 +12056,7 @@
         <v>Arrow Goby</v>
       </c>
     </row>
-    <row r="168" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A168" s="2">
         <v>904</v>
       </c>
@@ -12098,7 +12099,7 @@
         <v>Barred Surfperch</v>
       </c>
     </row>
-    <row r="169" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A169" s="2">
         <v>905</v>
       </c>
@@ -12141,7 +12142,7 @@
         <v>Bat Ray</v>
       </c>
     </row>
-    <row r="170" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A170" s="2">
         <v>906</v>
       </c>
@@ -12184,7 +12185,7 @@
         <v>Bay Goby</v>
       </c>
     </row>
-    <row r="171" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A171" s="2">
         <v>907</v>
       </c>
@@ -12227,7 +12228,7 @@
         <v>Bay Pipefish</v>
       </c>
     </row>
-    <row r="172" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A172" s="2">
         <v>908</v>
       </c>
@@ -12270,7 +12271,7 @@
         <v>Big Skate</v>
       </c>
     </row>
-    <row r="173" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A173" s="2">
         <v>909</v>
       </c>
@@ -12313,7 +12314,7 @@
         <v>Bigscale Logperch</v>
       </c>
     </row>
-    <row r="174" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A174" s="2">
         <v>910</v>
       </c>
@@ -12356,7 +12357,7 @@
         <v>Black Bass (unknown species)</v>
       </c>
     </row>
-    <row r="175" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A175" s="2">
         <v>911</v>
       </c>
@@ -12399,7 +12400,7 @@
         <v>Black Bullhead</v>
       </c>
     </row>
-    <row r="176" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A176" s="2">
         <v>912</v>
       </c>
@@ -12442,7 +12443,7 @@
         <v>Black Crappie</v>
       </c>
     </row>
-    <row r="177" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A177" s="2">
         <v>913</v>
       </c>
@@ -12485,7 +12486,7 @@
         <v>Blackfordia</v>
       </c>
     </row>
-    <row r="178" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A178" s="2">
         <v>914</v>
       </c>
@@ -12528,7 +12529,7 @@
         <v>Blue Catfish</v>
       </c>
     </row>
-    <row r="179" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A179" s="2">
         <v>915</v>
       </c>
@@ -12571,7 +12572,7 @@
         <v>Bluefin Killifish</v>
       </c>
     </row>
-    <row r="180" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A180" s="2">
         <v>916</v>
       </c>
@@ -12614,7 +12615,7 @@
         <v>Bluegill</v>
       </c>
     </row>
-    <row r="181" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A181" s="2">
         <v>917</v>
       </c>
@@ -12657,7 +12658,7 @@
         <v>Brown Bullhead</v>
       </c>
     </row>
-    <row r="182" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A182" s="2">
         <v>918</v>
       </c>
@@ -12700,7 +12701,7 @@
         <v>California Roach</v>
       </c>
     </row>
-    <row r="183" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A183" s="2">
         <v>919</v>
       </c>
@@ -12743,7 +12744,7 @@
         <v>Chameleon Goby</v>
       </c>
     </row>
-    <row r="184" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A184" s="2">
         <v>920</v>
       </c>
@@ -12786,7 +12787,7 @@
         <v>Channel Catfish</v>
       </c>
     </row>
-    <row r="185" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A185" s="2">
         <v>921</v>
       </c>
@@ -12829,7 +12830,7 @@
         <v>Chinook Salmon</v>
       </c>
     </row>
-    <row r="186" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A186" s="2">
         <v>922</v>
       </c>
@@ -12872,7 +12873,7 @@
         <v>Chrysaora</v>
       </c>
     </row>
-    <row r="187" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A187" s="2">
         <v>923</v>
       </c>
@@ -12915,7 +12916,7 @@
         <v>Comb Jelly</v>
       </c>
     </row>
-    <row r="188" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A188" s="2">
         <v>924</v>
       </c>
@@ -12958,7 +12959,7 @@
         <v>Common Carp</v>
       </c>
     </row>
-    <row r="189" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A189" s="2">
         <v>926</v>
       </c>
@@ -13001,7 +13002,7 @@
         <v>Crappie spp.</v>
       </c>
     </row>
-    <row r="190" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A190" s="2">
         <v>927</v>
       </c>
@@ -13044,7 +13045,7 @@
         <v>Cyprinid spp.</v>
       </c>
     </row>
-    <row r="191" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A191" s="2">
         <v>928</v>
       </c>
@@ -13087,7 +13088,7 @@
         <v>Delta Smelt</v>
       </c>
     </row>
-    <row r="192" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A192" s="2">
         <v>930</v>
       </c>
@@ -13130,7 +13131,7 @@
         <v>Fathead Minnow</v>
       </c>
     </row>
-    <row r="193" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A193" s="2">
         <v>931</v>
       </c>
@@ -13173,7 +13174,7 @@
         <v>Golden Shiner</v>
       </c>
     </row>
-    <row r="194" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A194" s="2">
         <v>932</v>
       </c>
@@ -13216,7 +13217,7 @@
         <v>Goldfish</v>
       </c>
     </row>
-    <row r="195" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A195" s="2">
         <v>933</v>
       </c>
@@ -13259,7 +13260,7 @@
         <v>Green Sturgeon</v>
       </c>
     </row>
-    <row r="196" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A196" s="2">
         <v>934</v>
       </c>
@@ -13302,7 +13303,7 @@
         <v>Green Sunfish</v>
       </c>
     </row>
-    <row r="197" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A197" s="2">
         <v>935</v>
       </c>
@@ -13345,7 +13346,7 @@
         <v>Hardhead</v>
       </c>
     </row>
-    <row r="198" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A198" s="2">
         <v>936</v>
       </c>
@@ -13388,7 +13389,7 @@
         <v>Harris Mud Crab</v>
       </c>
     </row>
-    <row r="199" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A199" s="2">
         <v>937</v>
       </c>
@@ -13431,7 +13432,7 @@
         <v>Hitch</v>
       </c>
     </row>
-    <row r="200" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A200" s="2">
         <v>938</v>
       </c>
@@ -13474,7 +13475,7 @@
         <v>Jacksmelt</v>
       </c>
     </row>
-    <row r="201" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A201" s="2">
         <v>939</v>
       </c>
@@ -13517,7 +13518,7 @@
         <v>Jellyfish Unid</v>
       </c>
     </row>
-    <row r="202" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A202" s="2">
         <v>940</v>
       </c>
@@ -13560,7 +13561,7 @@
         <v>Lamprey spp.</v>
       </c>
     </row>
-    <row r="203" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A203" s="2">
         <v>941</v>
       </c>
@@ -13603,7 +13604,7 @@
         <v>Largemouth Bass</v>
       </c>
     </row>
-    <row r="204" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A204" s="2">
         <v>942</v>
       </c>
@@ -13646,7 +13647,7 @@
         <v>Longfin Smelt</v>
       </c>
     </row>
-    <row r="205" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A205" s="2">
         <v>943</v>
       </c>
@@ -13689,7 +13690,7 @@
         <v>Maeotias</v>
       </c>
     </row>
-    <row r="206" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A206" s="2">
         <v>946</v>
       </c>
@@ -13732,7 +13733,7 @@
         <v>Moon Jellyfish</v>
       </c>
     </row>
-    <row r="207" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A207" s="2">
         <v>949</v>
       </c>
@@ -13775,7 +13776,7 @@
         <v>Northern Anchovy</v>
       </c>
     </row>
-    <row r="208" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A208" s="2">
         <v>950</v>
       </c>
@@ -13818,7 +13819,7 @@
         <v>Osmeridae spp.</v>
       </c>
     </row>
-    <row r="209" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A209" s="2">
         <v>951</v>
       </c>
@@ -13861,7 +13862,7 @@
         <v>Pacific Herring</v>
       </c>
     </row>
-    <row r="210" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A210" s="2">
         <v>952</v>
       </c>
@@ -13904,7 +13905,7 @@
         <v>Pacific Lamprey</v>
       </c>
     </row>
-    <row r="211" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A211" s="2">
         <v>953</v>
       </c>
@@ -13947,7 +13948,7 @@
         <v>Pacific Staghorn Sculpin</v>
       </c>
     </row>
-    <row r="212" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A212" s="2">
         <v>955</v>
       </c>
@@ -13990,7 +13991,7 @@
         <v>Plainfin Midshipman</v>
       </c>
     </row>
-    <row r="213" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A213" s="2">
         <v>956</v>
       </c>
@@ -14033,7 +14034,7 @@
         <v>Polyorchis</v>
       </c>
     </row>
-    <row r="214" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A214" s="2">
         <v>958</v>
       </c>
@@ -14076,7 +14077,7 @@
         <v>Pumpkinseed</v>
       </c>
     </row>
-    <row r="215" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A215" s="2">
         <v>960</v>
       </c>
@@ -14119,7 +14120,7 @@
         <v>Red Shiner</v>
       </c>
     </row>
-    <row r="216" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A216" s="2">
         <v>961</v>
       </c>
@@ -14162,7 +14163,7 @@
         <v>Redear</v>
       </c>
     </row>
-    <row r="217" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A217" s="2">
         <v>962</v>
       </c>
@@ -14205,7 +14206,7 @@
         <v>Redeye Bass</v>
       </c>
     </row>
-    <row r="218" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A218" s="2">
         <v>963</v>
       </c>
@@ -14248,7 +14249,7 @@
         <v>Riffle Sculpin</v>
       </c>
     </row>
-    <row r="219" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A219" s="2">
         <v>964</v>
       </c>
@@ -14291,7 +14292,7 @@
         <v>River Lamprey</v>
       </c>
     </row>
-    <row r="220" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A220" s="2">
         <v>965</v>
       </c>
@@ -14334,7 +14335,7 @@
         <v>Sacramento Blackfish</v>
       </c>
     </row>
-    <row r="221" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A221" s="2">
         <v>966</v>
       </c>
@@ -14377,7 +14378,7 @@
         <v>Sacramento Perch</v>
       </c>
     </row>
-    <row r="222" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A222" s="2">
         <v>967</v>
       </c>
@@ -14420,7 +14421,7 @@
         <v>Sacramento Pikeminnow</v>
       </c>
     </row>
-    <row r="223" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A223" s="2">
         <v>969</v>
       </c>
@@ -14463,7 +14464,7 @@
         <v>Scrippsia</v>
       </c>
     </row>
-    <row r="224" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A224" s="2">
         <v>970</v>
       </c>
@@ -14506,7 +14507,7 @@
         <v>Shimofuri Goby</v>
       </c>
     </row>
-    <row r="225" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A225" s="2">
         <v>971</v>
       </c>
@@ -14549,7 +14550,7 @@
         <v>Shokihaze Goby</v>
       </c>
     </row>
-    <row r="226" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A226" s="2">
         <v>972</v>
       </c>
@@ -14592,7 +14593,7 @@
         <v>Smallmouth Bass</v>
       </c>
     </row>
-    <row r="227" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A227" s="2">
         <v>973</v>
       </c>
@@ -14635,7 +14636,7 @@
         <v>Speckled Dace</v>
       </c>
     </row>
-    <row r="228" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A228" s="2">
         <v>974</v>
       </c>
@@ -14678,7 +14679,7 @@
         <v>Splittail</v>
       </c>
     </row>
-    <row r="229" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A229" s="2">
         <v>975</v>
       </c>
@@ -14721,7 +14722,7 @@
         <v>Spotted Bass</v>
       </c>
     </row>
-    <row r="230" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A230" s="2">
         <v>976</v>
       </c>
@@ -14764,7 +14765,7 @@
         <v>Starry Flounder</v>
       </c>
     </row>
-    <row r="231" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A231" s="2">
         <v>977</v>
       </c>
@@ -14807,7 +14808,7 @@
         <v>Steelhead</v>
       </c>
     </row>
-    <row r="232" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A232" s="2">
         <v>979</v>
       </c>
@@ -14850,7 +14851,7 @@
         <v>Sunfish (unknown species)</v>
       </c>
     </row>
-    <row r="233" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A233" s="2">
         <v>980</v>
       </c>
@@ -14893,7 +14894,7 @@
         <v>Surf Smelt</v>
       </c>
     </row>
-    <row r="234" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A234" s="2">
         <v>981</v>
       </c>
@@ -14936,7 +14937,7 @@
         <v>Threadfin Shad</v>
       </c>
     </row>
-    <row r="235" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A235" s="2">
         <v>982</v>
       </c>
@@ -14979,7 +14980,7 @@
         <v>Threespine Stickleback</v>
       </c>
     </row>
-    <row r="236" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A236" s="2">
         <v>983</v>
       </c>
@@ -15022,7 +15023,7 @@
         <v>Topsmelt</v>
       </c>
     </row>
-    <row r="237" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A237" s="2">
         <v>984</v>
       </c>
@@ -15065,7 +15066,7 @@
         <v>Tridentiger Spp.</v>
       </c>
     </row>
-    <row r="238" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A238" s="2">
         <v>985</v>
       </c>
@@ -15108,7 +15109,7 @@
         <v>Tule Perch</v>
       </c>
     </row>
-    <row r="239" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A239" s="2">
         <v>987</v>
       </c>
@@ -15151,7 +15152,7 @@
         <v>Wakasagi</v>
       </c>
     </row>
-    <row r="240" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A240" s="2">
         <v>988</v>
       </c>
@@ -15194,7 +15195,7 @@
         <v>Warmouth</v>
       </c>
     </row>
-    <row r="241" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A241" s="2">
         <v>989</v>
       </c>
@@ -15237,7 +15238,7 @@
         <v>White Catfish</v>
       </c>
     </row>
-    <row r="242" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A242" s="2">
         <v>990</v>
       </c>
@@ -15280,7 +15281,7 @@
         <v>White Crappie</v>
       </c>
     </row>
-    <row r="243" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A243" s="2">
         <v>991</v>
       </c>
@@ -15323,7 +15324,7 @@
         <v>White Croaker</v>
       </c>
     </row>
-    <row r="244" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A244" s="2">
         <v>992</v>
       </c>
@@ -15366,7 +15367,7 @@
         <v>White Sturgeon</v>
       </c>
     </row>
-    <row r="245" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A245" s="2">
         <v>993</v>
       </c>
@@ -15409,7 +15410,7 @@
         <v>Yellow Bullhead</v>
       </c>
     </row>
-    <row r="246" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A246" s="2">
         <v>994</v>
       </c>
@@ -15452,7 +15453,7 @@
         <v>Yellowfin Goby</v>
       </c>
     </row>
-    <row r="247" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A247" s="2">
         <v>77</v>
       </c>
@@ -15496,7 +15497,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="248" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A248" s="2">
         <v>110</v>
       </c>
@@ -15541,7 +15542,7 @@
         <v>Crangonyx</v>
       </c>
     </row>
-    <row r="249" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A249" s="2">
         <v>111</v>
       </c>
@@ -15586,7 +15587,7 @@
         <v>Hyalella</v>
       </c>
     </row>
-    <row r="250" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A250" s="2">
         <v>246</v>
       </c>
@@ -15631,7 +15632,7 @@
         <v>Grandidierella</v>
       </c>
     </row>
-    <row r="251" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A251" s="2">
         <v>253</v>
       </c>
@@ -15675,7 +15676,7 @@
         <v>1363</v>
       </c>
     </row>
-    <row r="252" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A252" s="2">
         <v>254</v>
       </c>
@@ -15719,7 +15720,7 @@
         <v>1363</v>
       </c>
     </row>
-    <row r="253" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A253" s="2">
         <v>303</v>
       </c>
@@ -15763,7 +15764,7 @@
         <v>1370</v>
       </c>
     </row>
-    <row r="254" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A254" s="2">
         <v>10000</v>
       </c>
@@ -15808,7 +15809,7 @@
         <v>Eogammarus</v>
       </c>
     </row>
-    <row r="255" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A255" s="2">
         <v>10018</v>
       </c>
@@ -15843,17 +15844,17 @@
         <v>0</v>
       </c>
       <c r="L255" t="s">
-        <v>140</v>
+        <v>246</v>
       </c>
       <c r="M255" t="s">
-        <v>139</v>
+        <v>32</v>
       </c>
       <c r="N255" t="str">
         <f t="shared" si="7"/>
         <v>Hydrobiidae</v>
       </c>
     </row>
-    <row r="256" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A256" s="2">
         <v>142</v>
       </c>
@@ -15898,7 +15899,7 @@
         <v>Fluminicola</v>
       </c>
     </row>
-    <row r="257" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A257" s="2">
         <v>143</v>
       </c>
@@ -15943,7 +15944,7 @@
         <v>Gyraulus</v>
       </c>
     </row>
-    <row r="258" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A258" s="2">
         <v>144</v>
       </c>
@@ -15988,7 +15989,7 @@
         <v>Melanoides tuberculata</v>
       </c>
     </row>
-    <row r="259" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A259" s="2">
         <v>154</v>
       </c>
@@ -16033,7 +16034,7 @@
         <v>Snail Other</v>
       </c>
     </row>
-    <row r="260" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A260" s="2">
         <v>166</v>
       </c>
@@ -16077,7 +16078,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="261" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A261" s="2">
         <v>169</v>
       </c>
@@ -16122,7 +16123,7 @@
         <v>Physa</v>
       </c>
     </row>
-    <row r="262" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A262" s="2">
         <v>170</v>
       </c>
@@ -16167,7 +16168,7 @@
         <v>Planorbella</v>
       </c>
     </row>
-    <row r="263" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A263" s="2">
         <v>172</v>
       </c>
@@ -16211,7 +16212,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="264" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A264" s="2">
         <v>185</v>
       </c>
@@ -16256,7 +16257,7 @@
         <v>Fossaria</v>
       </c>
     </row>
-    <row r="265" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A265" s="2">
         <v>189</v>
       </c>
@@ -16301,7 +16302,7 @@
         <v>Lymnaea</v>
       </c>
     </row>
-    <row r="266" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A266" s="2">
         <v>200</v>
       </c>
@@ -16346,7 +16347,7 @@
         <v>limpet</v>
       </c>
     </row>
-    <row r="267" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A267" s="2">
         <v>214</v>
       </c>
@@ -16390,7 +16391,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="268" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A268" s="2">
         <v>260</v>
       </c>
@@ -16434,7 +16435,7 @@
         <v>1353</v>
       </c>
     </row>
-    <row r="269" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A269" s="2">
         <v>10019</v>
       </c>
@@ -16478,7 +16479,7 @@
         <v>1332</v>
       </c>
     </row>
-    <row r="270" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A270" s="2">
         <v>900</v>
       </c>
@@ -16519,7 +16520,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="271" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A271" s="2">
         <v>59</v>
       </c>
@@ -16563,7 +16564,7 @@
         <v>1371</v>
       </c>
     </row>
-    <row r="272" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A272" s="2">
         <v>120</v>
       </c>
@@ -16607,7 +16608,7 @@
         <v>1372</v>
       </c>
     </row>
-    <row r="273" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A273" s="2">
         <v>121</v>
       </c>
@@ -16652,7 +16653,7 @@
         <v>Belostomatidae</v>
       </c>
     </row>
-    <row r="274" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A274" s="2">
         <v>122</v>
       </c>
@@ -16697,7 +16698,7 @@
         <v>Corixidae</v>
       </c>
     </row>
-    <row r="275" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A275" s="2">
         <v>123</v>
       </c>
@@ -16742,7 +16743,7 @@
         <v>Gerridae</v>
       </c>
     </row>
-    <row r="276" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A276" s="2">
         <v>124</v>
       </c>
@@ -16787,7 +16788,7 @@
         <v>Hydrometridae</v>
       </c>
     </row>
-    <row r="277" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A277" s="2">
         <v>125</v>
       </c>
@@ -16832,7 +16833,7 @@
         <v>Mesoveliidae</v>
       </c>
     </row>
-    <row r="278" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A278" s="2">
         <v>126</v>
       </c>
@@ -16877,7 +16878,7 @@
         <v>Vellidae</v>
       </c>
     </row>
-    <row r="279" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A279" s="2">
         <v>127</v>
       </c>
@@ -16922,7 +16923,7 @@
         <v>Hemiptera Other</v>
       </c>
     </row>
-    <row r="280" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A280" s="2">
         <v>159</v>
       </c>
@@ -16966,7 +16967,7 @@
         <v>1372</v>
       </c>
     </row>
-    <row r="281" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A281" s="2">
         <v>161</v>
       </c>
@@ -17010,7 +17011,7 @@
         <v>1372</v>
       </c>
     </row>
-    <row r="282" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A282" s="2">
         <v>237</v>
       </c>
@@ -17055,7 +17056,7 @@
         <v>Psyllidae</v>
       </c>
     </row>
-    <row r="283" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A283" s="2">
         <v>240</v>
       </c>
@@ -17100,7 +17101,7 @@
         <v>Hebridae</v>
       </c>
     </row>
-    <row r="284" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A284" s="2">
         <v>244</v>
       </c>
@@ -17145,7 +17146,7 @@
         <v>Nepidae</v>
       </c>
     </row>
-    <row r="285" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A285" s="2">
         <v>10009</v>
       </c>
@@ -17190,7 +17191,7 @@
         <v>Homoptera</v>
       </c>
     </row>
-    <row r="286" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A286" s="2">
         <v>10016</v>
       </c>
@@ -17234,7 +17235,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="287" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A287" s="2">
         <v>10017</v>
       </c>
@@ -17279,7 +17280,7 @@
         <v>Talitridae</v>
       </c>
     </row>
-    <row r="288" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A288" s="2">
         <v>901</v>
       </c>
@@ -17320,7 +17321,7 @@
         <v>1353</v>
       </c>
     </row>
-    <row r="289" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A289" s="2">
         <v>103</v>
       </c>
@@ -17364,7 +17365,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="290" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A290" s="2">
         <v>128</v>
       </c>
@@ -17409,7 +17410,7 @@
         <v>Hymenoptera Other</v>
       </c>
     </row>
-    <row r="291" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A291" s="2">
         <v>73</v>
       </c>
@@ -17453,7 +17454,7 @@
         <v>1375</v>
       </c>
     </row>
-    <row r="292" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A292" s="2">
         <v>178</v>
       </c>
@@ -17498,7 +17499,7 @@
         <v>Gnorimosphaeroma</v>
       </c>
     </row>
-    <row r="293" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A293" s="2">
         <v>184</v>
       </c>
@@ -17543,7 +17544,7 @@
         <v>Asellus</v>
       </c>
     </row>
-    <row r="294" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A294" s="2">
         <v>315</v>
       </c>
@@ -17588,7 +17589,7 @@
         <v>Ligidium</v>
       </c>
     </row>
-    <row r="295" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A295" s="2">
         <v>10001</v>
       </c>
@@ -17633,7 +17634,7 @@
         <v>Caecidotea</v>
       </c>
     </row>
-    <row r="296" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A296" s="2">
         <v>10004</v>
       </c>
@@ -17678,7 +17679,7 @@
         <v>Munnidae</v>
       </c>
     </row>
-    <row r="297" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A297" s="2">
         <v>10005</v>
       </c>
@@ -17723,7 +17724,7 @@
         <v>Isopod other</v>
       </c>
     </row>
-    <row r="298" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A298" s="2">
         <v>10008</v>
       </c>
@@ -17767,7 +17768,7 @@
         <v>1375</v>
       </c>
     </row>
-    <row r="299" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A299" s="2">
         <v>163</v>
       </c>
@@ -17811,7 +17812,7 @@
         <v>1353</v>
       </c>
     </row>
-    <row r="300" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A300" s="2">
         <v>10014</v>
       </c>
@@ -17855,7 +17856,7 @@
         <v>1353</v>
       </c>
     </row>
-    <row r="301" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A301" s="2">
         <v>13</v>
       </c>
@@ -17900,7 +17901,7 @@
         <v>Acanthomysis aspera</v>
       </c>
     </row>
-    <row r="302" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A302" s="2">
         <v>14</v>
       </c>
@@ -17945,7 +17946,7 @@
         <v>Acanthomysis bowmani</v>
       </c>
     </row>
-    <row r="303" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A303" s="2">
         <v>15</v>
       </c>
@@ -17990,7 +17991,7 @@
         <v>Acanthomysis hwanhaiensis</v>
       </c>
     </row>
-    <row r="304" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A304" s="2">
         <v>16</v>
       </c>
@@ -18035,7 +18036,7 @@
         <v>Acanthomysis macropsis</v>
       </c>
     </row>
-    <row r="305" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A305" s="2">
         <v>17</v>
       </c>
@@ -18080,7 +18081,7 @@
         <v>Deltamysis homquistae</v>
       </c>
     </row>
-    <row r="306" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A306" s="2">
         <v>18</v>
       </c>
@@ -18125,7 +18126,7 @@
         <v>Neomysis kadiakensis</v>
       </c>
     </row>
-    <row r="307" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A307" s="2">
         <v>19</v>
       </c>
@@ -18170,7 +18171,7 @@
         <v>Neomysis mercedis</v>
       </c>
     </row>
-    <row r="308" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A308" s="2">
         <v>71</v>
       </c>
@@ -18215,7 +18216,7 @@
         <v>Mysid Other</v>
       </c>
     </row>
-    <row r="309" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A309" s="2">
         <v>225</v>
       </c>
@@ -18260,7 +18261,7 @@
         <v>Mysid juvenile</v>
       </c>
     </row>
-    <row r="310" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A310" s="2">
         <v>226</v>
       </c>
@@ -18305,7 +18306,7 @@
         <v>Hyperacanthomysis longirostris</v>
       </c>
     </row>
-    <row r="311" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A311" s="2">
         <v>145</v>
       </c>
@@ -18349,7 +18350,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="312" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A312" s="2">
         <v>146</v>
       </c>
@@ -18393,7 +18394,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="313" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A313" s="2">
         <v>241</v>
       </c>
@@ -18437,7 +18438,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="314" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A314" s="2">
         <v>223</v>
       </c>
@@ -18481,7 +18482,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="315" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A315" s="2">
         <v>209</v>
       </c>
@@ -18526,7 +18527,7 @@
         <v>Gomphidae larvae</v>
       </c>
     </row>
-    <row r="316" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A316" s="2">
         <v>228</v>
       </c>
@@ -18571,7 +18572,7 @@
         <v>Zygoptera Adult</v>
       </c>
     </row>
-    <row r="317" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A317" s="2">
         <v>129</v>
       </c>
@@ -18616,7 +18617,7 @@
         <v>Aeshnidae larvae</v>
       </c>
     </row>
-    <row r="318" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A318" s="2">
         <v>130</v>
       </c>
@@ -18661,7 +18662,7 @@
         <v>Coenagrionidae larvae</v>
       </c>
     </row>
-    <row r="319" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A319" s="2">
         <v>131</v>
       </c>
@@ -18706,7 +18707,7 @@
         <v>Odonata Other</v>
       </c>
     </row>
-    <row r="320" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A320" s="2">
         <v>181</v>
       </c>
@@ -18751,7 +18752,7 @@
         <v>Libellulidae</v>
       </c>
     </row>
-    <row r="321" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A321" s="2">
         <v>191</v>
       </c>
@@ -18796,7 +18797,7 @@
         <v>Orthoptera</v>
       </c>
     </row>
-    <row r="322" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A322" s="2">
         <v>10</v>
       </c>
@@ -18841,7 +18842,7 @@
         <v>Ostracods</v>
       </c>
     </row>
-    <row r="323" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A323" s="2">
         <v>4</v>
       </c>
@@ -18886,7 +18887,7 @@
         <v>Insect larvae Other</v>
       </c>
     </row>
-    <row r="324" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A324" s="2">
         <v>11</v>
       </c>
@@ -18931,7 +18932,7 @@
         <v>Barnacle Nauplii</v>
       </c>
     </row>
-    <row r="325" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A325" s="2">
         <v>12</v>
       </c>
@@ -18976,7 +18977,7 @@
         <v>Copepod Nauplii</v>
       </c>
     </row>
-    <row r="326" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A326" s="2">
         <v>79</v>
       </c>
@@ -19021,7 +19022,7 @@
         <v>Malcostraca Other</v>
       </c>
     </row>
-    <row r="327" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A327" s="2">
         <v>95</v>
       </c>
@@ -19066,7 +19067,7 @@
         <v>Stomach/Gut Tissue</v>
       </c>
     </row>
-    <row r="328" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A328" s="2">
         <v>96</v>
       </c>
@@ -19111,7 +19112,7 @@
         <v>Debris (sand/silt/mud)</v>
       </c>
     </row>
-    <row r="329" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A329" s="2">
         <v>97</v>
       </c>
@@ -19156,7 +19157,7 @@
         <v>Plant material UNID</v>
       </c>
     </row>
-    <row r="330" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A330" s="2">
         <v>98</v>
       </c>
@@ -19201,7 +19202,7 @@
         <v>Animal material UNID</v>
       </c>
     </row>
-    <row r="331" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A331" s="2">
         <v>99</v>
       </c>
@@ -19246,7 +19247,7 @@
         <v>Zooplankton Other</v>
       </c>
     </row>
-    <row r="332" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A332" s="2">
         <v>135</v>
       </c>
@@ -19291,7 +19292,7 @@
         <v>Insect Unid</v>
       </c>
     </row>
-    <row r="333" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A333" s="2">
         <v>148</v>
       </c>
@@ -19336,7 +19337,7 @@
         <v>Eggs UNID</v>
       </c>
     </row>
-    <row r="334" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A334" s="2">
         <v>151</v>
       </c>
@@ -19381,7 +19382,7 @@
         <v>Copepod UNID</v>
       </c>
     </row>
-    <row r="335" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A335" s="2">
         <v>162</v>
       </c>
@@ -19426,7 +19427,7 @@
         <v>Egg Sacs</v>
       </c>
     </row>
-    <row r="336" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A336" s="2">
         <v>196</v>
       </c>
@@ -19471,7 +19472,7 @@
         <v>Tardigrade</v>
       </c>
     </row>
-    <row r="337" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A337" s="2">
         <v>222</v>
       </c>
@@ -19516,7 +19517,7 @@
         <v>Invertebrate UNID</v>
       </c>
     </row>
-    <row r="338" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A338" s="2">
         <v>312</v>
       </c>
@@ -19561,7 +19562,7 @@
         <v>Parasitic Copepod</v>
       </c>
     </row>
-    <row r="339" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A339" s="2">
         <v>400</v>
       </c>
@@ -19596,7 +19597,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="340" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A340" s="2">
         <v>401</v>
       </c>
@@ -19631,7 +19632,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="341" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A341" s="2">
         <v>402</v>
       </c>
@@ -19666,7 +19667,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="342" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A342" s="2">
         <v>403</v>
       </c>
@@ -19701,7 +19702,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="343" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A343" s="2">
         <v>404</v>
       </c>
@@ -19736,7 +19737,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="344" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A344" s="2">
         <v>405</v>
       </c>
@@ -19771,7 +19772,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="345" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A345" s="2">
         <v>406</v>
       </c>
@@ -19806,7 +19807,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="346" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A346" s="2">
         <v>407</v>
       </c>
@@ -19841,7 +19842,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="347" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A347" s="2">
         <v>408</v>
       </c>
@@ -19876,7 +19877,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="348" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A348" s="2">
         <v>409</v>
       </c>
@@ -19911,7 +19912,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="349" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A349" s="2">
         <v>410</v>
       </c>
@@ -19946,7 +19947,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="350" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A350" s="2">
         <v>411</v>
       </c>
@@ -19981,7 +19982,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="351" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A351" s="2">
         <v>412</v>
       </c>
@@ -20016,7 +20017,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="352" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A352" s="2">
         <v>413</v>
       </c>
@@ -20051,7 +20052,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="353" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A353" s="2">
         <v>414</v>
       </c>
@@ -20086,7 +20087,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="354" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A354" s="2">
         <v>415</v>
       </c>
@@ -20121,7 +20122,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="355" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A355" s="2">
         <v>416</v>
       </c>
@@ -20156,7 +20157,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="356" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A356" s="2">
         <v>417</v>
       </c>
@@ -20191,7 +20192,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="357" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A357" s="2">
         <v>418</v>
       </c>
@@ -20226,7 +20227,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="358" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A358" s="2">
         <v>419</v>
       </c>
@@ -20261,7 +20262,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="359" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A359" s="2">
         <v>420</v>
       </c>
@@ -20296,7 +20297,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="360" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A360" s="2">
         <v>421</v>
       </c>
@@ -20331,7 +20332,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="361" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A361" s="2">
         <v>422</v>
       </c>
@@ -20366,7 +20367,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="362" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A362" s="2">
         <v>423</v>
       </c>
@@ -20401,7 +20402,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="363" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A363" s="2">
         <v>424</v>
       </c>
@@ -20436,7 +20437,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="364" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A364" s="2">
         <v>425</v>
       </c>
@@ -20471,7 +20472,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="365" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A365" s="2">
         <v>426</v>
       </c>
@@ -20506,7 +20507,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="366" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A366" s="2">
         <v>427</v>
       </c>
@@ -20541,7 +20542,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="367" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:13" ht="72" x14ac:dyDescent="0.3">
       <c r="A367" s="2">
         <v>428</v>
       </c>
@@ -20576,7 +20577,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="368" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:13" ht="72" x14ac:dyDescent="0.3">
       <c r="A368" s="2">
         <v>429</v>
       </c>
@@ -20611,7 +20612,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="369" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A369" s="2">
         <v>430</v>
       </c>
@@ -20646,7 +20647,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="370" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A370" s="2">
         <v>431</v>
       </c>
@@ -20681,7 +20682,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="371" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A371" s="2">
         <v>432</v>
       </c>
@@ -20716,7 +20717,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="372" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A372" s="2">
         <v>433</v>
       </c>
@@ -20751,7 +20752,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="373" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A373" s="2">
         <v>434</v>
       </c>
@@ -20786,7 +20787,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="374" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A374" s="2">
         <v>435</v>
       </c>
@@ -20821,7 +20822,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="375" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A375" s="2">
         <v>436</v>
       </c>
@@ -20856,7 +20857,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="376" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A376" s="2">
         <v>437</v>
       </c>
@@ -20891,7 +20892,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="377" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A377" s="2">
         <v>438</v>
       </c>
@@ -20926,7 +20927,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="378" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A378" s="2">
         <v>439</v>
       </c>
@@ -20961,7 +20962,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="379" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A379" s="2">
         <v>440</v>
       </c>
@@ -20996,7 +20997,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="380" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A380" s="2">
         <v>441</v>
       </c>
@@ -21031,7 +21032,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="381" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A381" s="2">
         <v>442</v>
       </c>
@@ -21066,7 +21067,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="382" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A382" s="2">
         <v>443</v>
       </c>
@@ -21101,7 +21102,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="383" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A383" s="2">
         <v>444</v>
       </c>
@@ -21136,7 +21137,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="384" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A384" s="2">
         <v>445</v>
       </c>
@@ -21171,7 +21172,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="385" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A385" s="2">
         <v>446</v>
       </c>
@@ -21206,7 +21207,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="386" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A386" s="2">
         <v>447</v>
       </c>
@@ -21241,7 +21242,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="387" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A387" s="2">
         <v>448</v>
       </c>
@@ -21276,7 +21277,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="388" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A388" s="2">
         <v>449</v>
       </c>
@@ -21311,7 +21312,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="389" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A389" s="2">
         <v>450</v>
       </c>
@@ -21346,7 +21347,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="390" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A390" s="2">
         <v>451</v>
       </c>
@@ -21381,7 +21382,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="391" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A391" s="2">
         <v>452</v>
       </c>
@@ -21416,7 +21417,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="392" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A392" s="2">
         <v>453</v>
       </c>
@@ -21451,7 +21452,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="393" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="393" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A393" s="2">
         <v>454</v>
       </c>
@@ -21486,7 +21487,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="394" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="394" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A394" s="2">
         <v>455</v>
       </c>
@@ -21521,7 +21522,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="395" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A395" s="2">
         <v>456</v>
       </c>
@@ -21556,7 +21557,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="396" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A396" s="2">
         <v>457</v>
       </c>
@@ -21591,7 +21592,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="397" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A397" s="2">
         <v>458</v>
       </c>
@@ -21626,7 +21627,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="398" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A398" s="2">
         <v>459</v>
       </c>
@@ -21661,7 +21662,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="399" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A399" s="2">
         <v>460</v>
       </c>
@@ -21696,7 +21697,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="400" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A400" s="2">
         <v>461</v>
       </c>
@@ -21731,7 +21732,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="401" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="401" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A401" s="2">
         <v>462</v>
       </c>
@@ -21766,7 +21767,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="402" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="402" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A402" s="2">
         <v>463</v>
       </c>
@@ -21801,7 +21802,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="403" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="403" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A403" s="2">
         <v>464</v>
       </c>
@@ -21836,7 +21837,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="404" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="404" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A404" s="2">
         <v>465</v>
       </c>
@@ -21871,7 +21872,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="405" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="405" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A405" s="2">
         <v>466</v>
       </c>
@@ -21906,7 +21907,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="406" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="406" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A406" s="2">
         <v>467</v>
       </c>
@@ -21941,7 +21942,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="407" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="407" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A407" s="2">
         <v>468</v>
       </c>
@@ -21976,7 +21977,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="408" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="408" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A408" s="2">
         <v>469</v>
       </c>
@@ -22011,7 +22012,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="409" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="409" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A409" s="2">
         <v>470</v>
       </c>
@@ -22046,7 +22047,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="410" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="410" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A410" s="2">
         <v>471</v>
       </c>
@@ -22081,7 +22082,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="411" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="411" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A411" s="2">
         <v>472</v>
       </c>
@@ -22116,7 +22117,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="412" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="412" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A412" s="2">
         <v>473</v>
       </c>
@@ -22151,7 +22152,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="413" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="413" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A413" s="2">
         <v>474</v>
       </c>
@@ -22186,7 +22187,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="414" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="414" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A414" s="2">
         <v>475</v>
       </c>
@@ -22221,7 +22222,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="415" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="415" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A415" s="2">
         <v>476</v>
       </c>
@@ -22256,7 +22257,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="416" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="416" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A416" s="2">
         <v>477</v>
       </c>
@@ -22291,7 +22292,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="417" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="417" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A417" s="2">
         <v>478</v>
       </c>
@@ -22326,7 +22327,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="418" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="418" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A418" s="2">
         <v>479</v>
       </c>
@@ -22361,7 +22362,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="419" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="419" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A419" s="2">
         <v>480</v>
       </c>
@@ -22396,7 +22397,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="420" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="420" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A420" s="2">
         <v>481</v>
       </c>
@@ -22431,7 +22432,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="421" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="421" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A421" s="2">
         <v>482</v>
       </c>
@@ -22467,7 +22468,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="422" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="422" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A422" s="2">
         <v>483</v>
       </c>
@@ -22503,7 +22504,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="423" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="423" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A423" s="2">
         <v>484</v>
       </c>
@@ -22539,7 +22540,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="424" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="424" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A424" s="2">
         <v>485</v>
       </c>
@@ -22575,7 +22576,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="425" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="425" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A425" s="2">
         <v>486</v>
       </c>
@@ -22611,7 +22612,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="426" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="426" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A426" s="2">
         <v>487</v>
       </c>
@@ -22647,7 +22648,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="427" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="427" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A427" s="2">
         <v>488</v>
       </c>
@@ -22683,7 +22684,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="428" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="428" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A428" s="2">
         <v>489</v>
       </c>
@@ -22719,7 +22720,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="429" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="429" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A429" s="2">
         <v>490</v>
       </c>
@@ -22755,7 +22756,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="430" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="430" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A430" s="2">
         <v>491</v>
       </c>
@@ -22791,7 +22792,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="431" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="431" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A431" s="2">
         <v>492</v>
       </c>
@@ -22827,7 +22828,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="432" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="432" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A432" s="2">
         <v>493</v>
       </c>
@@ -22863,7 +22864,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="433" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="433" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A433" s="2">
         <v>494</v>
       </c>
@@ -22899,7 +22900,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="434" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="434" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A434" s="2">
         <v>495</v>
       </c>
@@ -22935,7 +22936,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="435" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="435" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A435" s="2">
         <v>496</v>
       </c>
@@ -22971,7 +22972,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="436" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="436" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A436" s="2">
         <v>497</v>
       </c>
@@ -23007,7 +23008,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="437" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="437" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A437" s="2">
         <v>498</v>
       </c>
@@ -23043,7 +23044,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="438" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="438" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A438" s="2">
         <v>499</v>
       </c>
@@ -23079,7 +23080,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="439" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="439" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A439" s="2">
         <v>500</v>
       </c>
@@ -23115,7 +23116,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="440" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="440" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A440" s="2">
         <v>501</v>
       </c>
@@ -23151,7 +23152,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="441" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="441" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A441" s="2">
         <v>502</v>
       </c>
@@ -23187,7 +23188,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="442" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="442" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A442" s="2">
         <v>503</v>
       </c>
@@ -23223,7 +23224,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="443" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="443" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A443" s="2">
         <v>504</v>
       </c>
@@ -23259,7 +23260,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="444" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="444" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A444" s="2">
         <v>505</v>
       </c>
@@ -23295,7 +23296,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="445" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="445" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A445" s="2">
         <v>506</v>
       </c>
@@ -23331,7 +23332,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="446" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="446" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A446" s="2">
         <v>507</v>
       </c>
@@ -23367,7 +23368,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="447" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="447" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A447" s="2">
         <v>508</v>
       </c>
@@ -23403,7 +23404,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="448" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="448" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A448" s="2">
         <v>509</v>
       </c>
@@ -23439,7 +23440,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="449" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="449" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A449" s="2">
         <v>510</v>
       </c>
@@ -23475,7 +23476,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="450" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="450" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A450" s="2">
         <v>511</v>
       </c>
@@ -23511,7 +23512,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="451" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="451" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A451" s="2">
         <v>512</v>
       </c>
@@ -23547,7 +23548,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="452" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="452" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A452" s="2">
         <v>513</v>
       </c>
@@ -23583,7 +23584,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="453" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="453" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A453" s="2">
         <v>514</v>
       </c>
@@ -23619,7 +23620,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="454" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="454" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A454" s="2">
         <v>515</v>
       </c>
@@ -23655,7 +23656,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="455" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="455" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A455" s="2">
         <v>516</v>
       </c>
@@ -23691,7 +23692,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="456" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="456" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A456" s="2">
         <v>517</v>
       </c>
@@ -23727,7 +23728,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="457" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="457" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A457" s="2">
         <v>518</v>
       </c>
@@ -23763,7 +23764,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="458" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="458" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A458" s="2">
         <v>519</v>
       </c>
@@ -23799,7 +23800,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="459" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="459" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A459" s="2">
         <v>520</v>
       </c>
@@ -23835,7 +23836,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="460" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="460" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A460" s="2">
         <v>521</v>
       </c>
@@ -23871,7 +23872,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="461" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="461" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A461" s="2">
         <v>522</v>
       </c>
@@ -23907,7 +23908,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="462" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="462" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A462" s="2">
         <v>523</v>
       </c>
@@ -23943,7 +23944,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="463" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="463" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A463" s="2">
         <v>524</v>
       </c>
@@ -23979,7 +23980,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="464" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="464" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A464" s="2">
         <v>525</v>
       </c>
@@ -24015,7 +24016,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="465" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="465" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A465" s="2">
         <v>526</v>
       </c>
@@ -24051,7 +24052,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="466" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="466" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A466" s="2">
         <v>527</v>
       </c>
@@ -24087,7 +24088,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="467" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="467" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A467" s="2">
         <v>528</v>
       </c>
@@ -24123,7 +24124,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="468" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="468" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A468" s="2">
         <v>529</v>
       </c>
@@ -24159,7 +24160,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="469" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="469" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A469" s="2">
         <v>530</v>
       </c>
@@ -24195,7 +24196,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="470" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="470" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A470" s="2">
         <v>531</v>
       </c>
@@ -24231,7 +24232,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="471" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="471" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A471" s="2">
         <v>532</v>
       </c>
@@ -24267,7 +24268,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="472" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="472" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A472" s="2">
         <v>533</v>
       </c>
@@ -24303,7 +24304,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="473" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="473" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A473" s="2">
         <v>534</v>
       </c>
@@ -24339,7 +24340,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="474" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="474" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A474" s="2">
         <v>535</v>
       </c>
@@ -24375,7 +24376,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="475" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="475" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A475" s="2">
         <v>536</v>
       </c>
@@ -24411,7 +24412,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="476" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="476" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A476" s="2">
         <v>537</v>
       </c>
@@ -24447,7 +24448,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="477" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="477" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A477" s="2">
         <v>538</v>
       </c>
@@ -24483,7 +24484,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="478" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="478" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A478" s="2">
         <v>539</v>
       </c>
@@ -24519,7 +24520,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="479" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="479" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A479" s="2">
         <v>540</v>
       </c>
@@ -24555,7 +24556,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="480" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="480" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A480" s="2">
         <v>541</v>
       </c>
@@ -24591,7 +24592,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="481" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="481" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A481" s="2">
         <v>542</v>
       </c>
@@ -24627,7 +24628,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="482" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="482" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A482" s="2">
         <v>543</v>
       </c>
@@ -24663,7 +24664,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="483" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="483" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A483" s="2">
         <v>544</v>
       </c>
@@ -24699,7 +24700,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="484" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="484" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A484" s="2">
         <v>545</v>
       </c>
@@ -24735,7 +24736,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="485" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="485" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A485" s="2">
         <v>546</v>
       </c>
@@ -24771,7 +24772,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="486" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="486" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A486" s="2">
         <v>547</v>
       </c>
@@ -24807,7 +24808,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="487" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="487" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A487" s="2">
         <v>548</v>
       </c>
@@ -24843,7 +24844,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="488" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="488" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A488" s="2">
         <v>549</v>
       </c>
@@ -24879,7 +24880,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="489" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="489" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A489" s="2">
         <v>550</v>
       </c>
@@ -24915,7 +24916,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="490" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="490" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A490" s="2">
         <v>557</v>
       </c>
@@ -24951,7 +24952,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="491" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="491" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A491" s="2">
         <v>559</v>
       </c>
@@ -24987,7 +24988,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="492" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="492" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A492" s="2">
         <v>564</v>
       </c>
@@ -25023,7 +25024,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="493" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="493" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A493" s="2">
         <v>565</v>
       </c>
@@ -25059,7 +25060,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="494" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="494" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A494" s="2">
         <v>566</v>
       </c>
@@ -25095,7 +25096,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="495" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="495" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A495" s="2">
         <v>574</v>
       </c>
@@ -25131,7 +25132,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="496" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="496" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A496" s="2">
         <v>575</v>
       </c>
@@ -25167,7 +25168,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="497" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="497" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A497" s="2">
         <v>576</v>
       </c>
@@ -25203,7 +25204,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="498" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="498" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A498" s="2">
         <v>577</v>
       </c>
@@ -25239,7 +25240,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="499" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="499" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A499" s="2">
         <v>578</v>
       </c>
@@ -25275,7 +25276,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="500" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="500" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A500" s="2">
         <v>147</v>
       </c>
@@ -25320,7 +25321,7 @@
         <v>Planaria</v>
       </c>
     </row>
-    <row r="501" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="501" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A501" s="2">
         <v>219</v>
       </c>
@@ -25364,7 +25365,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="502" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="502" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A502" s="2">
         <v>243</v>
       </c>
@@ -25408,7 +25409,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="503" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="503" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A503" s="2">
         <v>2</v>
       </c>
@@ -25452,7 +25453,7 @@
         <v>1360</v>
       </c>
     </row>
-    <row r="504" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="504" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A504" s="2">
         <v>7</v>
       </c>
@@ -25496,7 +25497,7 @@
         <v>1360</v>
       </c>
     </row>
-    <row r="505" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="505" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A505" s="2">
         <v>88</v>
       </c>
@@ -25540,7 +25541,7 @@
         <v>1360</v>
       </c>
     </row>
-    <row r="506" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="506" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A506" s="2">
         <v>89</v>
       </c>
@@ -25584,7 +25585,7 @@
         <v>1360</v>
       </c>
     </row>
-    <row r="507" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="507" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A507" s="2">
         <v>90</v>
       </c>
@@ -25628,7 +25629,7 @@
         <v>1360</v>
       </c>
     </row>
-    <row r="508" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="508" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A508" s="2">
         <v>91</v>
       </c>
@@ -25672,7 +25673,7 @@
         <v>1360</v>
       </c>
     </row>
-    <row r="509" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="509" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A509" s="2">
         <v>92</v>
       </c>
@@ -25716,7 +25717,7 @@
         <v>1360</v>
       </c>
     </row>
-    <row r="510" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="510" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A510" s="2">
         <v>93</v>
       </c>
@@ -25760,7 +25761,7 @@
         <v>1360</v>
       </c>
     </row>
-    <row r="511" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="511" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A511" s="2">
         <v>249</v>
       </c>
@@ -25804,7 +25805,7 @@
         <v>1360</v>
       </c>
     </row>
-    <row r="512" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="512" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A512" s="2">
         <v>256</v>
       </c>
@@ -25848,7 +25849,7 @@
         <v>1360</v>
       </c>
     </row>
-    <row r="513" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="513" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A513" s="2">
         <v>264</v>
       </c>
@@ -25892,7 +25893,7 @@
         <v>1360</v>
       </c>
     </row>
-    <row r="514" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="514" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A514" s="2">
         <v>800</v>
       </c>
@@ -25934,7 +25935,7 @@
         <v>1353</v>
       </c>
     </row>
-    <row r="515" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="515" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A515" s="2">
         <v>182</v>
       </c>
@@ -25979,7 +25980,7 @@
         <v>Tanaid</v>
       </c>
     </row>
-    <row r="516" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="516" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A516" s="2">
         <v>132</v>
       </c>
@@ -26024,7 +26025,7 @@
         <v>Thrips</v>
       </c>
     </row>
-    <row r="517" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="517" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A517" s="2">
         <v>133</v>
       </c>
@@ -26068,7 +26069,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="518" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="518" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A518" s="2">
         <v>134</v>
       </c>
@@ -26112,7 +26113,7 @@
         <v>1376</v>
       </c>
     </row>
-    <row r="519" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="519" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A519" s="2">
         <v>190</v>
       </c>
@@ -26156,7 +26157,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="520" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="520" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A520" s="2">
         <v>198</v>
       </c>
@@ -26201,7 +26202,7 @@
         <v>Polycentripodidae larvae</v>
       </c>
     </row>
-    <row r="521" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="521" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A521" s="2">
         <v>236</v>
       </c>
@@ -26245,7 +26246,7 @@
         <v>1376</v>
       </c>
     </row>
-    <row r="522" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="522" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A522" s="2">
         <v>9999</v>
       </c>
@@ -26282,7 +26283,7 @@
         <v>No Catch</v>
       </c>
     </row>
-    <row r="523" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="523" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A523" s="2">
         <v>10021</v>
       </c>
@@ -26327,7 +26328,7 @@
         <v>Psyllidae Larvae</v>
       </c>
     </row>
-    <row r="524" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="524" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A524" s="2">
         <v>10022</v>
       </c>
@@ -26372,7 +26373,7 @@
         <v>Tenebrionidae adult</v>
       </c>
     </row>
-    <row r="525" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="525" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A525" s="2">
         <v>10024</v>
       </c>
@@ -26417,7 +26418,7 @@
         <v>Coccinellidae Larvae</v>
       </c>
     </row>
-    <row r="526" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="526" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A526" s="2">
         <v>10025</v>
       </c>
@@ -26462,7 +26463,7 @@
         <v>Scirtidae adult</v>
       </c>
     </row>
-    <row r="527" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="527" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A527" s="2">
         <v>10026</v>
       </c>
@@ -26507,7 +26508,7 @@
         <v>Stratiomyidae</v>
       </c>
     </row>
-    <row r="528" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="528" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A528" s="2">
         <v>10028</v>
       </c>
@@ -26551,7 +26552,7 @@
         <v>1353</v>
       </c>
     </row>
-    <row r="529" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="529" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A529" s="2">
         <v>10029</v>
       </c>
@@ -26595,7 +26596,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="530" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="530" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A530" s="2">
         <v>11000</v>
       </c>
@@ -26653,16 +26654,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" customWidth="1"/>
+    <col min="1" max="1" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -26673,7 +26674,7 @@
         <v>1356</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>189</v>
       </c>
@@ -26684,7 +26685,7 @@
         <v>2.9359999999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>191</v>
       </c>
@@ -26695,7 +26696,7 @@
         <v>2.7446000000000002</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>138</v>
       </c>
@@ -26708,7 +26709,7 @@
         <v>3.0009999999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>141</v>
       </c>
@@ -26719,7 +26720,7 @@
         <v>3.0150000000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>1357</v>
       </c>
@@ -26730,7 +26731,7 @@
         <v>3.0150000000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>1300</v>
       </c>
@@ -26743,7 +26744,7 @@
         <v>3.0009999999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>267</v>
       </c>
@@ -26754,7 +26755,7 @@
         <v>3.0150000000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>193</v>
       </c>
@@ -26765,7 +26766,7 @@
         <v>3.0150000000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>490</v>
       </c>
@@ -26776,7 +26777,7 @@
         <v>3.0150000000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>488</v>
       </c>
@@ -26787,7 +26788,7 @@
         <v>3.0150000000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>485</v>
       </c>

</xml_diff>